<commit_message>
working trials, updated sheet
</commit_message>
<xml_diff>
--- a/trials.xlsx
+++ b/trials.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MEGASync\Projects\Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\djeeta-chan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,24 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="12">
   <si>
-    <t>Dark Trial</t>
-  </si>
-  <si>
-    <t>Fire Trial</t>
-  </si>
-  <si>
-    <t>Water Trial</t>
-  </si>
-  <si>
-    <t>Earth Trial</t>
-  </si>
-  <si>
-    <t>Wind Trial</t>
-  </si>
-  <si>
-    <t>Light Trial</t>
-  </si>
-  <si>
     <t>Vohu</t>
   </si>
   <si>
@@ -60,6 +42,24 @@
   </si>
   <si>
     <t>Cocy</t>
+  </si>
+  <si>
+    <t>Dark</t>
+  </si>
+  <si>
+    <t>Fire</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>Earth</t>
+  </si>
+  <si>
+    <t>Wind</t>
+  </si>
+  <si>
+    <t>Light</t>
   </si>
 </sst>
 </file>
@@ -414,8 +414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection sqref="A1:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,250 +426,250 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
         <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Trials fix, showdowns upgrade, sheet fix
</commit_message>
<xml_diff>
--- a/trials.xlsx
+++ b/trials.xlsx
@@ -41,9 +41,6 @@
     <t>Ifrit</t>
   </si>
   <si>
-    <t>Cocy</t>
-  </si>
-  <si>
     <t>Dark</t>
   </si>
   <si>
@@ -60,6 +57,9 @@
   </si>
   <si>
     <t>Light</t>
+  </si>
+  <si>
+    <t>Cocytus</t>
   </si>
 </sst>
 </file>
@@ -414,8 +414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection sqref="A1:A31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,7 +426,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -434,7 +434,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -442,7 +442,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -450,7 +450,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -458,7 +458,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -466,7 +466,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -474,7 +474,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
@@ -482,7 +482,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
@@ -490,7 +490,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
@@ -498,7 +498,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
@@ -506,7 +506,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
@@ -514,7 +514,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
@@ -522,7 +522,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
         <v>4</v>
@@ -530,7 +530,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
@@ -538,31 +538,31 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18" t="s">
         <v>1</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B19" t="s">
         <v>1</v>
@@ -578,7 +578,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20" t="s">
         <v>1</v>
@@ -586,7 +586,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B21" t="s">
         <v>0</v>
@@ -594,7 +594,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22" t="s">
         <v>0</v>
@@ -602,7 +602,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B23" t="s">
         <v>0</v>
@@ -610,7 +610,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24" t="s">
         <v>3</v>
@@ -618,7 +618,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B25" t="s">
         <v>3</v>
@@ -626,7 +626,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B26" t="s">
         <v>3</v>
@@ -634,7 +634,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
@@ -642,7 +642,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B28" t="s">
         <v>4</v>
@@ -650,7 +650,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B29" t="s">
         <v>4</v>
@@ -658,18 +658,18 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
turned off insults, updated sheet
</commit_message>
<xml_diff>
--- a/trials.xlsx
+++ b/trials.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="15">
   <si>
     <t>Dark</t>
   </si>
@@ -56,9 +56,6 @@
     <t>Corow &amp; Sagittarius</t>
   </si>
   <si>
-    <t>Diablo &amp; Sagittarius</t>
-  </si>
-  <si>
     <t>Vohu Manah &amp; Sagittarius</t>
   </si>
   <si>
@@ -68,10 +65,10 @@
     <t>Ifrit &amp; Cocytus</t>
   </si>
   <si>
-    <t>Corow</t>
-  </si>
-  <si>
-    <t>Ifrit &amp; Sagittarius</t>
+    <t>Diablo</t>
+  </si>
+  <si>
+    <t>Ifrit</t>
   </si>
 </sst>
 </file>
@@ -89,7 +86,10 @@
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -100,7 +100,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -109,38 +109,91 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color rgb="FF000000"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color rgb="FF000000"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
@@ -149,20 +202,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -477,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,255 +549,257 @@
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B15" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="B16" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="B17" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="B18" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B19" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="7" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated GW, event schedule, trials
</commit_message>
<xml_diff>
--- a/trials.xlsx
+++ b/trials.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="12">
   <si>
     <t>Dark</t>
   </si>
@@ -66,7 +66,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,6 +82,14 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -91,7 +99,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -99,20 +107,77 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -429,263 +494,268 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B7" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B19" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="31" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>2</v>
-      </c>
-      <c r="B27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>2</v>
-      </c>
-      <c r="B28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>3</v>
-      </c>
-      <c r="B30" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="3"/>
-    </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>